<commit_message>
process scenario frequencies and write to file
</commit_message>
<xml_diff>
--- a/input/similarity_c_c_binary_m.xlsx
+++ b/input/similarity_c_c_binary_m.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LocalUserData\User-data\feita1\Uni\PhD\Projects\French keyboard\Optimization\optimizing-the-french-keyboard\input\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035"/>
   </bookViews>
@@ -244,12 +249,6 @@
   </si>
   <si>
     <t>≃</t>
-  </si>
-  <si>
-    <t>⩽</t>
-  </si>
-  <si>
-    <t>⩾</t>
   </si>
   <si>
     <t>¤</t>
@@ -545,6 +544,12 @@
   <si>
     <t>Ω</t>
   </si>
+  <si>
+    <t>≤</t>
+  </si>
+  <si>
+    <t>≥</t>
+  </si>
 </sst>
 </file>
 
@@ -629,6 +634,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -676,7 +684,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -711,7 +719,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -922,8 +930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FU177"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="B1:K1048576"/>
+    <sheetView tabSelected="1" topLeftCell="AS1" workbookViewId="0">
+      <selection activeCell="CA1" sqref="CA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1164,304 +1172,304 @@
         <v>75</v>
       </c>
       <c r="BZ1" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="CA1" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="CB1" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="CA1" s="3" t="s">
+      <c r="CC1" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="CB1" s="3" t="s">
+      <c r="CD1" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="CC1" s="3" t="s">
+      <c r="CE1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="CD1" s="3" t="s">
+      <c r="CF1" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="CE1" s="3" t="s">
+      <c r="CG1" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="CF1" s="3" t="s">
+      <c r="CH1" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="CG1" s="3" t="s">
+      <c r="CI1" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="CH1" s="3" t="s">
+      <c r="CJ1" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="CI1" s="3" t="s">
+      <c r="CK1" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="CJ1" s="3" t="s">
+      <c r="CL1" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="CK1" s="3" t="s">
+      <c r="CM1" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="CL1" s="3" t="s">
+      <c r="CN1" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="CM1" s="3" t="s">
+      <c r="CO1" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="CN1" s="3" t="s">
+      <c r="CP1" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="CO1" s="3" t="s">
+      <c r="CQ1" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="CP1" s="3" t="s">
+      <c r="CR1" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="CQ1" s="3" t="s">
+      <c r="CS1" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="CR1" s="3" t="s">
+      <c r="CT1" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="CS1" s="3" t="s">
+      <c r="CU1" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="CT1" s="3" t="s">
+      <c r="CV1" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="CU1" s="3" t="s">
+      <c r="CW1" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="CV1" s="3" t="s">
+      <c r="CX1" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="CW1" s="3" t="s">
+      <c r="CY1" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="CX1" s="3" t="s">
+      <c r="CZ1" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="CY1" s="3" t="s">
+      <c r="DA1" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="CZ1" s="3" t="s">
+      <c r="DB1" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="DA1" s="3" t="s">
+      <c r="DC1" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="DB1" s="3" t="s">
+      <c r="DD1" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="DC1" s="3" t="s">
+      <c r="DE1" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="DD1" s="3" t="s">
+      <c r="DF1" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="DE1" s="3" t="s">
+      <c r="DG1" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="DF1" s="3" t="s">
+      <c r="DH1" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="DG1" s="3" t="s">
+      <c r="DI1" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="DH1" s="3" t="s">
+      <c r="DJ1" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="DI1" s="3" t="s">
+      <c r="DK1" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="DJ1" s="3" t="s">
+      <c r="DL1" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="DK1" s="3" t="s">
+      <c r="DM1" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="DL1" s="3" t="s">
+      <c r="DN1" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="DM1" s="3" t="s">
+      <c r="DO1" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="DN1" s="3" t="s">
+      <c r="DP1" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="DO1" s="3" t="s">
+      <c r="DQ1" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="DP1" s="3" t="s">
+      <c r="DR1" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="DQ1" s="3" t="s">
+      <c r="DS1" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="DR1" s="3" t="s">
+      <c r="DT1" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="DS1" s="3" t="s">
+      <c r="DU1" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="DT1" s="3" t="s">
+      <c r="DV1" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="DU1" s="3" t="s">
+      <c r="DW1" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="DV1" s="3" t="s">
+      <c r="DX1" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="DW1" s="3" t="s">
+      <c r="DY1" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="DX1" s="3" t="s">
+      <c r="DZ1" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="DY1" s="3" t="s">
+      <c r="EA1" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="DZ1" s="3" t="s">
+      <c r="EB1" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="EA1" s="3" t="s">
+      <c r="EC1" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="EB1" s="3" t="s">
+      <c r="ED1" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="EC1" s="3" t="s">
+      <c r="EE1" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="ED1" s="3" t="s">
+      <c r="EF1" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="EE1" s="3" t="s">
+      <c r="EG1" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="EF1" s="3" t="s">
+      <c r="EH1" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="EG1" s="3" t="s">
+      <c r="EI1" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="EH1" s="3" t="s">
+      <c r="EJ1" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="EI1" s="3" t="s">
+      <c r="EK1" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="EJ1" s="3" t="s">
+      <c r="EL1" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="EK1" s="3" t="s">
+      <c r="EM1" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="EL1" s="3" t="s">
+      <c r="EN1" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="EM1" s="3" t="s">
+      <c r="EO1" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="EN1" s="3" t="s">
+      <c r="EP1" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="EO1" s="3" t="s">
+      <c r="EQ1" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="EP1" s="3" t="s">
+      <c r="ER1" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="EQ1" s="3" t="s">
+      <c r="ES1" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="ER1" s="3" t="s">
+      <c r="ET1" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="ES1" s="3" t="s">
+      <c r="EU1" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="ET1" s="3" t="s">
+      <c r="EV1" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="EU1" s="3" t="s">
+      <c r="EW1" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="EV1" s="3" t="s">
+      <c r="EX1" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="EW1" s="3" t="s">
+      <c r="EY1" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="EX1" s="3" t="s">
+      <c r="EZ1" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="EY1" s="3" t="s">
+      <c r="FA1" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="EZ1" s="3" t="s">
+      <c r="FB1" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="FA1" s="3" t="s">
+      <c r="FC1" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="FB1" s="3" t="s">
+      <c r="FD1" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="FC1" s="3" t="s">
+      <c r="FE1" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="FD1" s="3" t="s">
+      <c r="FF1" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="FE1" s="3" t="s">
+      <c r="FG1" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="FF1" s="3" t="s">
+      <c r="FH1" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="FG1" s="3" t="s">
+      <c r="FI1" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="FH1" s="3" t="s">
+      <c r="FJ1" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="FI1" s="3" t="s">
+      <c r="FK1" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="FJ1" s="3" t="s">
+      <c r="FL1" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="FK1" s="3" t="s">
+      <c r="FM1" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="FL1" s="3" t="s">
+      <c r="FN1" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="FM1" s="3" t="s">
+      <c r="FO1" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="FN1" s="3" t="s">
+      <c r="FP1" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="FO1" s="3" t="s">
+      <c r="FQ1" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="FP1" s="3" t="s">
+      <c r="FR1" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="FQ1" s="3" t="s">
+      <c r="FS1" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="FR1" s="3" t="s">
+      <c r="FT1" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="FS1" s="3" t="s">
+      <c r="FU1" s="3" t="s">
         <v>173</v>
-      </c>
-      <c r="FT1" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="FU1" s="3" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:177" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -15346,7 +15354,7 @@
     </row>
     <row r="78" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
-        <v>76</v>
+        <v>174</v>
       </c>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
@@ -15529,7 +15537,7 @@
     </row>
     <row r="79" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
-        <v>77</v>
+        <v>175</v>
       </c>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
@@ -15710,7 +15718,7 @@
     </row>
     <row r="80" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
@@ -15891,7 +15899,7 @@
     </row>
     <row r="81" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
@@ -16074,7 +16082,7 @@
     </row>
     <row r="82" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
@@ -16257,7 +16265,7 @@
     </row>
     <row r="83" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
@@ -16440,7 +16448,7 @@
     </row>
     <row r="84" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
@@ -16623,7 +16631,7 @@
     </row>
     <row r="85" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
@@ -16806,7 +16814,7 @@
     </row>
     <row r="86" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
@@ -16987,7 +16995,7 @@
     </row>
     <row r="87" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
@@ -17172,7 +17180,7 @@
     </row>
     <row r="88" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
@@ -17355,7 +17363,7 @@
     </row>
     <row r="89" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
@@ -17536,7 +17544,7 @@
     </row>
     <row r="90" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
@@ -17717,7 +17725,7 @@
     </row>
     <row r="91" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
@@ -17900,7 +17908,7 @@
     </row>
     <row r="92" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
@@ -18081,7 +18089,7 @@
     </row>
     <row r="93" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
@@ -18264,7 +18272,7 @@
     </row>
     <row r="94" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
@@ -18445,7 +18453,7 @@
     </row>
     <row r="95" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B95" s="3"/>
       <c r="C95" s="3"/>
@@ -18628,7 +18636,7 @@
     </row>
     <row r="96" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>
@@ -18809,7 +18817,7 @@
     </row>
     <row r="97" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B97" s="3"/>
       <c r="C97" s="3"/>
@@ -18992,7 +19000,7 @@
     </row>
     <row r="98" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B98" s="3"/>
       <c r="C98" s="3"/>
@@ -19173,7 +19181,7 @@
     </row>
     <row r="99" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B99" s="3"/>
       <c r="C99" s="3"/>
@@ -19354,7 +19362,7 @@
     </row>
     <row r="100" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
@@ -19535,7 +19543,7 @@
     </row>
     <row r="101" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
@@ -19716,7 +19724,7 @@
     </row>
     <row r="102" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B102" s="3"/>
       <c r="C102" s="3"/>
@@ -19897,7 +19905,7 @@
     </row>
     <row r="103" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
@@ -20078,7 +20086,7 @@
     </row>
     <row r="104" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B104" s="3"/>
       <c r="C104" s="3"/>
@@ -20259,7 +20267,7 @@
     </row>
     <row r="105" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B105" s="3"/>
       <c r="C105" s="3"/>
@@ -20440,7 +20448,7 @@
     </row>
     <row r="106" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B106" s="3"/>
       <c r="C106" s="3"/>
@@ -20623,7 +20631,7 @@
     </row>
     <row r="107" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B107" s="3"/>
       <c r="C107" s="3"/>
@@ -20804,7 +20812,7 @@
     </row>
     <row r="108" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B108" s="3"/>
       <c r="C108" s="3"/>
@@ -20987,7 +20995,7 @@
     </row>
     <row r="109" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B109" s="3"/>
       <c r="C109" s="3"/>
@@ -21168,7 +21176,7 @@
     </row>
     <row r="110" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
@@ -21351,7 +21359,7 @@
     </row>
     <row r="111" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
@@ -21532,7 +21540,7 @@
     </row>
     <row r="112" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B112" s="3"/>
       <c r="C112" s="3"/>
@@ -21715,7 +21723,7 @@
     </row>
     <row r="113" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
@@ -21898,7 +21906,7 @@
     </row>
     <row r="114" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B114" s="3"/>
       <c r="C114" s="3"/>
@@ -22079,7 +22087,7 @@
     </row>
     <row r="115" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B115" s="3"/>
       <c r="C115" s="3"/>
@@ -22260,7 +22268,7 @@
     </row>
     <row r="116" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B116" s="3"/>
       <c r="C116" s="3"/>
@@ -22443,7 +22451,7 @@
     </row>
     <row r="117" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B117" s="3"/>
       <c r="C117" s="3"/>
@@ -22624,7 +22632,7 @@
     </row>
     <row r="118" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B118" s="3"/>
       <c r="C118" s="3"/>
@@ -22805,7 +22813,7 @@
     </row>
     <row r="119" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B119" s="3"/>
       <c r="C119" s="3"/>
@@ -22988,7 +22996,7 @@
     </row>
     <row r="120" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B120" s="3"/>
       <c r="C120" s="3"/>
@@ -23169,7 +23177,7 @@
     </row>
     <row r="121" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B121" s="3"/>
       <c r="C121" s="3"/>
@@ -23350,7 +23358,7 @@
     </row>
     <row r="122" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B122" s="3"/>
       <c r="C122" s="3"/>
@@ -23533,7 +23541,7 @@
     </row>
     <row r="123" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B123" s="3"/>
       <c r="C123" s="3"/>
@@ -23714,7 +23722,7 @@
     </row>
     <row r="124" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B124" s="3"/>
       <c r="C124" s="3"/>
@@ -23895,7 +23903,7 @@
     </row>
     <row r="125" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B125" s="3"/>
       <c r="C125" s="3"/>
@@ -24078,7 +24086,7 @@
     </row>
     <row r="126" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B126" s="3"/>
       <c r="C126" s="3"/>
@@ -24259,7 +24267,7 @@
     </row>
     <row r="127" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B127" s="3"/>
       <c r="C127" s="3"/>
@@ -24442,7 +24450,7 @@
     </row>
     <row r="128" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B128" s="3"/>
       <c r="C128" s="3"/>
@@ -24623,7 +24631,7 @@
     </row>
     <row r="129" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B129" s="3"/>
       <c r="C129" s="3"/>
@@ -24806,7 +24814,7 @@
     </row>
     <row r="130" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B130" s="3"/>
       <c r="C130" s="3"/>
@@ -24987,7 +24995,7 @@
     </row>
     <row r="131" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B131" s="3"/>
       <c r="C131" s="3"/>
@@ -25170,7 +25178,7 @@
     </row>
     <row r="132" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A132" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B132" s="3"/>
       <c r="C132" s="3"/>
@@ -25351,7 +25359,7 @@
     </row>
     <row r="133" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B133" s="3"/>
       <c r="C133" s="3"/>
@@ -25534,7 +25542,7 @@
     </row>
     <row r="134" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B134" s="3"/>
       <c r="C134" s="3"/>
@@ -25715,7 +25723,7 @@
     </row>
     <row r="135" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B135" s="3"/>
       <c r="C135" s="3"/>
@@ -25898,7 +25906,7 @@
     </row>
     <row r="136" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B136" s="3"/>
       <c r="C136" s="3"/>
@@ -26079,7 +26087,7 @@
     </row>
     <row r="137" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B137" s="3"/>
       <c r="C137" s="3"/>
@@ -26262,7 +26270,7 @@
     </row>
     <row r="138" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B138" s="3"/>
       <c r="C138" s="3"/>
@@ -26443,7 +26451,7 @@
     </row>
     <row r="139" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B139" s="3"/>
       <c r="C139" s="3"/>
@@ -26626,7 +26634,7 @@
     </row>
     <row r="140" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A140" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B140" s="3"/>
       <c r="C140" s="3"/>
@@ -26807,7 +26815,7 @@
     </row>
     <row r="141" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B141" s="3"/>
       <c r="C141" s="3"/>
@@ -26990,7 +26998,7 @@
     </row>
     <row r="142" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B142" s="3"/>
       <c r="C142" s="3"/>
@@ -27171,7 +27179,7 @@
     </row>
     <row r="143" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B143" s="3"/>
       <c r="C143" s="3"/>
@@ -27356,7 +27364,7 @@
     </row>
     <row r="144" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B144" s="3"/>
       <c r="C144" s="3"/>
@@ -27537,7 +27545,7 @@
     </row>
     <row r="145" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A145" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B145" s="3"/>
       <c r="C145" s="3"/>
@@ -27718,7 +27726,7 @@
     </row>
     <row r="146" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A146" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B146" s="3"/>
       <c r="C146" s="3"/>
@@ -27901,7 +27909,7 @@
     </row>
     <row r="147" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A147" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B147" s="3"/>
       <c r="C147" s="3"/>
@@ -28082,7 +28090,7 @@
     </row>
     <row r="148" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B148" s="3"/>
       <c r="C148" s="3"/>
@@ -28265,7 +28273,7 @@
     </row>
     <row r="149" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B149" s="3"/>
       <c r="C149" s="3"/>
@@ -28446,7 +28454,7 @@
     </row>
     <row r="150" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A150" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B150" s="3"/>
       <c r="C150" s="3"/>
@@ -28629,7 +28637,7 @@
     </row>
     <row r="151" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B151" s="3"/>
       <c r="C151" s="3"/>
@@ -28810,7 +28818,7 @@
     </row>
     <row r="152" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B152" s="3"/>
       <c r="C152" s="3"/>
@@ -28993,7 +29001,7 @@
     </row>
     <row r="153" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A153" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B153" s="3"/>
       <c r="C153" s="3"/>
@@ -29174,7 +29182,7 @@
     </row>
     <row r="154" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A154" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B154" s="3"/>
       <c r="C154" s="3"/>
@@ -29357,7 +29365,7 @@
     </row>
     <row r="155" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A155" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B155" s="3"/>
       <c r="C155" s="3"/>
@@ -29538,7 +29546,7 @@
     </row>
     <row r="156" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A156" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B156" s="3"/>
       <c r="C156" s="3"/>
@@ -29721,7 +29729,7 @@
     </row>
     <row r="157" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A157" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B157" s="3"/>
       <c r="C157" s="3"/>
@@ -29902,7 +29910,7 @@
     </row>
     <row r="158" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B158" s="3"/>
       <c r="C158" s="3"/>
@@ -30085,7 +30093,7 @@
     </row>
     <row r="159" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B159" s="3"/>
       <c r="C159" s="3"/>
@@ -30266,7 +30274,7 @@
     </row>
     <row r="160" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B160" s="3"/>
       <c r="C160" s="3"/>
@@ -30449,7 +30457,7 @@
     </row>
     <row r="161" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A161" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B161" s="3"/>
       <c r="C161" s="3"/>
@@ -30630,7 +30638,7 @@
     </row>
     <row r="162" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A162" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B162" s="3"/>
       <c r="C162" s="3"/>
@@ -30813,7 +30821,7 @@
     </row>
     <row r="163" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A163" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B163" s="3"/>
       <c r="C163" s="3"/>
@@ -30994,7 +31002,7 @@
     </row>
     <row r="164" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A164" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B164" s="3"/>
       <c r="C164" s="3"/>
@@ -31177,7 +31185,7 @@
     </row>
     <row r="165" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B165" s="3"/>
       <c r="C165" s="3"/>
@@ -31358,7 +31366,7 @@
     </row>
     <row r="166" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B166" s="3"/>
       <c r="C166" s="3"/>
@@ -31541,7 +31549,7 @@
     </row>
     <row r="167" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B167" s="3"/>
       <c r="C167" s="3"/>
@@ -31722,7 +31730,7 @@
     </row>
     <row r="168" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B168" s="3"/>
       <c r="C168" s="3"/>
@@ -31905,7 +31913,7 @@
     </row>
     <row r="169" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A169" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B169" s="3"/>
       <c r="C169" s="3"/>
@@ -32086,7 +32094,7 @@
     </row>
     <row r="170" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A170" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B170" s="3"/>
       <c r="C170" s="3"/>
@@ -32269,7 +32277,7 @@
     </row>
     <row r="171" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A171" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B171" s="3"/>
       <c r="C171" s="3"/>
@@ -32450,7 +32458,7 @@
     </row>
     <row r="172" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A172" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B172" s="3"/>
       <c r="C172" s="3"/>
@@ -32633,7 +32641,7 @@
     </row>
     <row r="173" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B173" s="3"/>
       <c r="C173" s="3"/>
@@ -32814,7 +32822,7 @@
     </row>
     <row r="174" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A174" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B174" s="3"/>
       <c r="C174" s="3"/>
@@ -32997,7 +33005,7 @@
     </row>
     <row r="175" spans="1:177" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B175" s="3"/>
       <c r="C175" s="3"/>
@@ -33178,7 +33186,7 @@
     </row>
     <row r="176" spans="1:177" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A176" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B176" s="3"/>
       <c r="C176" s="3"/>
@@ -33361,7 +33369,7 @@
     </row>
     <row r="177" spans="1:177" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A177" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B177" s="3"/>
       <c r="C177" s="3"/>

</xml_diff>